<commit_message>
new campaing scenarios and excel added
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/KampanyaTestleri.xlsx
+++ b/src/test/resources/excel/KampanyaTestleri.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27706"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gratisit-my.sharepoint.com/personal/engk01tr_gratis_com_tr/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BCC8B2A7-7164-47DC-8492-0E6D8C24D981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{502575F6-1FF1-47FA-B00B-43434EEC1C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="8" activeTab="8" xr2:uid="{0087B5A3-399B-4A17-8A95-DF6F2C9CFF5C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="9" activeTab="10" xr2:uid="{0087B5A3-399B-4A17-8A95-DF6F2C9CFF5C}"/>
   </bookViews>
   <sheets>
     <sheet name="1022310223" sheetId="5" r:id="rId1"/>
@@ -21,8 +21,9 @@
     <sheet name="1022110221" sheetId="3" r:id="rId6"/>
     <sheet name="1022610226" sheetId="9" r:id="rId7"/>
     <sheet name="1022010220" sheetId="14" r:id="rId8"/>
-    <sheet name="1024910249" sheetId="4" r:id="rId9"/>
-    <sheet name="1025510255" sheetId="13" r:id="rId10"/>
+    <sheet name="1025510255" sheetId="13" r:id="rId9"/>
+    <sheet name="1024910249" sheetId="4" r:id="rId10"/>
+    <sheet name="1031510315" sheetId="15" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="23">
   <si>
     <t>Ürün Kodu</t>
   </si>
@@ -76,12 +77,51 @@
   <si>
     <t>MT</t>
   </si>
+  <si>
+    <t>812.64</t>
+  </si>
+  <si>
+    <t>81.26</t>
+  </si>
+  <si>
+    <t>731.38</t>
+  </si>
+  <si>
+    <t>599.25</t>
+  </si>
+  <si>
+    <t>59.93</t>
+  </si>
+  <si>
+    <t>539.32</t>
+  </si>
+  <si>
+    <t>582.5</t>
+  </si>
+  <si>
+    <t>58.25</t>
+  </si>
+  <si>
+    <t>524.25</t>
+  </si>
+  <si>
+    <t>868.99</t>
+  </si>
+  <si>
+    <t>86.9</t>
+  </si>
+  <si>
+    <t>782.09</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MT </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,8 +155,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,6 +180,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4B084"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -148,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -183,10 +234,20 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -918,14 +979,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="D11:D15"/>
-    <mergeCell ref="E11:E15"/>
-    <mergeCell ref="F11:F15"/>
-    <mergeCell ref="B2:B9"/>
-    <mergeCell ref="C2:C9"/>
-    <mergeCell ref="D2:D9"/>
-    <mergeCell ref="E2:E9"/>
-    <mergeCell ref="F2:F9"/>
     <mergeCell ref="G17:G22"/>
     <mergeCell ref="G24:G32"/>
     <mergeCell ref="G2:G9"/>
@@ -942,17 +995,25 @@
     <mergeCell ref="F24:F32"/>
     <mergeCell ref="B11:B15"/>
     <mergeCell ref="C11:C15"/>
+    <mergeCell ref="D11:D15"/>
+    <mergeCell ref="E11:E15"/>
+    <mergeCell ref="F11:F15"/>
+    <mergeCell ref="B2:B9"/>
+    <mergeCell ref="C2:C9"/>
+    <mergeCell ref="D2:D9"/>
+    <mergeCell ref="E2:E9"/>
+    <mergeCell ref="F2:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32994263-25BE-40BB-935D-F1983009F224}">
-  <dimension ref="A1:G124"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6A820D7-2A77-47D5-9EF4-EA2F91DD3F2E}">
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -990,160 +1051,148 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="7">
-        <v>10023698</v>
+      <c r="A2" s="2">
+        <v>10029055</v>
       </c>
       <c r="B2" s="12">
-        <v>394.99</v>
-      </c>
-      <c r="C2" s="14">
-        <v>36.840000000000003</v>
-      </c>
-      <c r="D2" s="14">
-        <v>358.15</v>
+        <v>399.5</v>
+      </c>
+      <c r="C2" s="12">
+        <v>33.5</v>
+      </c>
+      <c r="D2" s="12">
+        <v>366</v>
       </c>
       <c r="E2" s="12">
         <v>0</v>
       </c>
       <c r="F2" s="12">
-        <v>358.15</v>
+        <v>366</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="7">
-        <v>10018762</v>
+      <c r="A3" s="2">
+        <v>10016979</v>
       </c>
       <c r="B3" s="12"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="7">
-        <v>10003482</v>
+      <c r="A4" s="2">
+        <v>10016981</v>
       </c>
       <c r="B4" s="12"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="7">
-        <v>10003450</v>
+      <c r="A5" s="2">
+        <v>10017022</v>
       </c>
       <c r="B5" s="12"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="7">
-        <v>13000295</v>
+      <c r="A6" s="2">
+        <v>10029636</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
     </row>
-    <row r="7" spans="1:7" ht="15.6">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.6">
-      <c r="A8" s="6">
-        <v>10018762</v>
-      </c>
-      <c r="B8" s="12">
-        <v>326.5</v>
-      </c>
-      <c r="C8" s="13">
-        <v>31.15</v>
-      </c>
-      <c r="D8" s="13">
-        <v>295.35000000000002</v>
-      </c>
-      <c r="E8" s="12">
-        <v>34.9</v>
-      </c>
-      <c r="F8" s="12">
-        <v>330.25</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.6">
-      <c r="A9" s="6">
-        <v>10015790</v>
+    <row r="7" spans="1:7">
+      <c r="A7" s="2">
+        <v>10029636</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="2">
+        <v>10033046</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="2">
+        <v>10017090</v>
       </c>
       <c r="B9" s="12"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
     </row>
-    <row r="10" spans="1:7" ht="15.6">
-      <c r="A10" s="6">
-        <v>13000295</v>
-      </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
+    <row r="10" spans="1:7">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11"/>
+      <c r="A11" s="2">
+        <v>10031016</v>
+      </c>
+      <c r="B11" s="12">
+        <v>228.5</v>
+      </c>
+      <c r="C11" s="12">
+        <v>33.5</v>
+      </c>
+      <c r="D11" s="12">
+        <v>195</v>
+      </c>
+      <c r="E11" s="12">
+        <v>34.9</v>
+      </c>
+      <c r="F11" s="12">
+        <v>229.9</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="2">
-        <v>10003480</v>
-      </c>
-      <c r="B12" s="12">
-        <v>434.49</v>
-      </c>
-      <c r="C12" s="12">
-        <v>36.840000000000003</v>
-      </c>
-      <c r="D12" s="12">
-        <v>397.65</v>
-      </c>
-      <c r="E12" s="12">
-        <v>0</v>
-      </c>
-      <c r="F12" s="12">
-        <v>397.65</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>9</v>
-      </c>
+        <v>10029055</v>
+      </c>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="2">
-        <v>10017642</v>
+        <v>10029055</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
@@ -1154,7 +1203,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="2">
-        <v>10003450</v>
+        <v>10005052</v>
       </c>
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
@@ -1165,7 +1214,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="2">
-        <v>13000295</v>
+        <v>10005052</v>
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
@@ -1175,37 +1224,30 @@
       <c r="G15" s="12"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16"/>
+      <c r="A16" s="2">
+        <v>10014863</v>
+      </c>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="2">
-        <v>10015247</v>
-      </c>
-      <c r="B17" s="12">
-        <v>897.48</v>
-      </c>
-      <c r="C17" s="12">
-        <v>73.680000000000007</v>
-      </c>
-      <c r="D17" s="12">
-        <v>823.8</v>
-      </c>
-      <c r="E17" s="12">
-        <v>0</v>
-      </c>
-      <c r="F17" s="12">
-        <v>823.8</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>7</v>
-      </c>
+        <v>10029636</v>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="2">
-        <v>10017003</v>
+        <v>10029636</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -1215,30 +1257,37 @@
       <c r="G18" s="12"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="2">
-        <v>10003450</v>
-      </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
+      <c r="A19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="2">
-        <v>10003450</v>
-      </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
+        <v>10006676</v>
+      </c>
+      <c r="B20" s="12">
+        <v>217.75</v>
+      </c>
+      <c r="C20" s="12">
+        <v>16.75</v>
+      </c>
+      <c r="D20" s="12">
+        <v>201</v>
+      </c>
+      <c r="E20" s="12">
+        <v>0</v>
+      </c>
+      <c r="F20" s="12">
+        <v>201</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="2">
-        <v>13000295</v>
+        <v>10005104</v>
       </c>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
@@ -1249,7 +1298,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="2">
-        <v>13000295</v>
+        <v>10029052</v>
       </c>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
@@ -1260,7 +1309,7 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="2">
-        <v>10023194</v>
+        <v>10005052</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
@@ -1271,7 +1320,7 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="2">
-        <v>10023190</v>
+        <v>10022377</v>
       </c>
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
@@ -1281,37 +1330,30 @@
       <c r="G24" s="12"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G25"/>
+      <c r="A25" s="2">
+        <v>10014863</v>
+      </c>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="2">
-        <v>10015790</v>
-      </c>
-      <c r="B26" s="12">
-        <v>614.98</v>
-      </c>
-      <c r="C26" s="12">
-        <v>42.53</v>
-      </c>
-      <c r="D26" s="12">
-        <v>572.45000000000005</v>
-      </c>
-      <c r="E26" s="12">
-        <v>0</v>
-      </c>
-      <c r="F26" s="12">
-        <v>572.45000000000005</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>7</v>
-      </c>
+        <v>10029636</v>
+      </c>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="2">
-        <v>10014865</v>
+        <v>10008866</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
@@ -1321,30 +1363,37 @@
       <c r="G27" s="12"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="2">
-        <v>10028562</v>
-      </c>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
+      <c r="A28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="2">
-        <v>10004378</v>
-      </c>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
+        <v>10021661</v>
+      </c>
+      <c r="B29" s="12">
+        <v>1707</v>
+      </c>
+      <c r="C29" s="12">
+        <v>33.5</v>
+      </c>
+      <c r="D29" s="12">
+        <v>1673.5</v>
+      </c>
+      <c r="E29" s="12">
+        <v>0</v>
+      </c>
+      <c r="F29" s="12">
+        <v>1673.5</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="2">
-        <v>10003450</v>
+        <v>10002298</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
@@ -1355,7 +1404,7 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="2">
-        <v>10003450</v>
+        <v>10029636</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
@@ -1366,7 +1415,7 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="2">
-        <v>13000295</v>
+        <v>10029636</v>
       </c>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
@@ -1377,7 +1426,7 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="2">
-        <v>10015188</v>
+        <v>10001399</v>
       </c>
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
@@ -1387,59 +1436,59 @@
       <c r="G33" s="12"/>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G34"/>
+      <c r="A34" s="2">
+        <v>10019602</v>
+      </c>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="2">
-        <v>10028783</v>
-      </c>
-      <c r="B35" s="12">
-        <v>1451.48</v>
-      </c>
-      <c r="C35" s="12">
-        <v>104.83</v>
-      </c>
-      <c r="D35" s="12">
-        <v>1346.65</v>
-      </c>
-      <c r="E35" s="12">
-        <v>0</v>
-      </c>
-      <c r="F35" s="12">
-        <v>1346.65</v>
-      </c>
-      <c r="G35" s="12" t="s">
-        <v>9</v>
-      </c>
+        <v>10003352</v>
+      </c>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="2">
-        <v>10019034</v>
-      </c>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
+      <c r="A36" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36"/>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="2">
-        <v>10003450</v>
-      </c>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
+        <v>10031016</v>
+      </c>
+      <c r="B37" s="12">
+        <v>251.75</v>
+      </c>
+      <c r="C37" s="12">
+        <v>16.75</v>
+      </c>
+      <c r="D37" s="12">
+        <v>235</v>
+      </c>
+      <c r="E37" s="12">
+        <v>34.9</v>
+      </c>
+      <c r="F37" s="12">
+        <v>269.89999999999998</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="2">
-        <v>10003450</v>
+        <v>10015790</v>
       </c>
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
@@ -1450,7 +1499,7 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="2">
-        <v>13000295</v>
+        <v>10002298</v>
       </c>
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
@@ -1461,7 +1510,7 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="2">
-        <v>13000295</v>
+        <v>10029636</v>
       </c>
       <c r="B40" s="12"/>
       <c r="C40" s="12"/>
@@ -1472,7 +1521,7 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="2">
-        <v>13000295</v>
+        <v>10001399</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="12"/>
@@ -1483,7 +1532,7 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="2">
-        <v>14000119</v>
+        <v>10001399</v>
       </c>
       <c r="B42" s="12"/>
       <c r="C42" s="12"/>
@@ -1492,38 +1541,38 @@
       <c r="F42" s="12"/>
       <c r="G42" s="12"/>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" ht="15">
       <c r="A43" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G43"/>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" ht="15">
       <c r="A44" s="2">
         <v>10029636</v>
       </c>
       <c r="B44" s="12">
-        <v>549.24</v>
+        <v>1534</v>
       </c>
       <c r="C44" s="12">
-        <v>36.840000000000003</v>
+        <v>16.75</v>
       </c>
       <c r="D44" s="12">
-        <v>512.4</v>
+        <v>1517.25</v>
       </c>
       <c r="E44" s="12">
         <v>0</v>
       </c>
       <c r="F44" s="12">
-        <v>512.4</v>
+        <v>1517.25</v>
       </c>
       <c r="G44" s="12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15">
       <c r="A45" s="2">
-        <v>10033046</v>
+        <v>10015566</v>
       </c>
       <c r="B45" s="12"/>
       <c r="C45" s="12"/>
@@ -1532,9 +1581,9 @@
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" ht="14.45" customHeight="1">
       <c r="A46" s="2">
-        <v>10003450</v>
+        <v>10033046</v>
       </c>
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
@@ -1543,9 +1592,9 @@
       <c r="F46" s="12"/>
       <c r="G46" s="12"/>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" ht="14.45" customHeight="1">
       <c r="A47" s="2">
-        <v>13000295</v>
+        <v>10011403</v>
       </c>
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
@@ -1554,38 +1603,31 @@
       <c r="F47" s="12"/>
       <c r="G47" s="12"/>
     </row>
-    <row r="48" spans="1:7">
-      <c r="A48" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G48"/>
-    </row>
-    <row r="49" spans="1:7">
+    <row r="48" spans="1:7" ht="14.45" customHeight="1">
+      <c r="A48" s="2">
+        <v>14000119</v>
+      </c>
+      <c r="B48" s="12"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+    </row>
+    <row r="49" spans="1:7" ht="14.45" customHeight="1">
       <c r="A49" s="2">
-        <v>10023698</v>
-      </c>
-      <c r="B49" s="12">
-        <v>331</v>
-      </c>
-      <c r="C49" s="12">
-        <v>31.15</v>
-      </c>
-      <c r="D49" s="12">
-        <v>299.85000000000002</v>
-      </c>
-      <c r="E49" s="12">
-        <v>34.9</v>
-      </c>
-      <c r="F49" s="12">
-        <v>334.75</v>
-      </c>
-      <c r="G49" s="12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7">
+        <v>14000119</v>
+      </c>
+      <c r="B49" s="12"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+    </row>
+    <row r="50" spans="1:7" ht="14.45" customHeight="1">
       <c r="A50" s="2">
-        <v>10003480</v>
+        <v>10011355</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
@@ -1594,9 +1636,9 @@
       <c r="F50" s="12"/>
       <c r="G50" s="12"/>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" ht="14.45" customHeight="1">
       <c r="A51" s="2">
-        <v>13000295</v>
+        <v>10003352</v>
       </c>
       <c r="B51" s="12"/>
       <c r="C51" s="12"/>
@@ -1605,673 +1647,495 @@
       <c r="F51" s="12"/>
       <c r="G51" s="12"/>
     </row>
-    <row r="52" spans="1:7">
-      <c r="A52" s="2" t="s">
+    <row r="52" spans="1:7" ht="15"/>
+  </sheetData>
+  <mergeCells count="36">
+    <mergeCell ref="G44:G51"/>
+    <mergeCell ref="B44:B51"/>
+    <mergeCell ref="C44:C51"/>
+    <mergeCell ref="D44:D51"/>
+    <mergeCell ref="E44:E51"/>
+    <mergeCell ref="F44:F51"/>
+    <mergeCell ref="G29:G35"/>
+    <mergeCell ref="G37:G42"/>
+    <mergeCell ref="G2:G9"/>
+    <mergeCell ref="G11:G18"/>
+    <mergeCell ref="G20:G27"/>
+    <mergeCell ref="B37:B42"/>
+    <mergeCell ref="C37:C42"/>
+    <mergeCell ref="D37:D42"/>
+    <mergeCell ref="E37:E42"/>
+    <mergeCell ref="F37:F42"/>
+    <mergeCell ref="B29:B35"/>
+    <mergeCell ref="C29:C35"/>
+    <mergeCell ref="D29:D35"/>
+    <mergeCell ref="E29:E35"/>
+    <mergeCell ref="F29:F35"/>
+    <mergeCell ref="B11:B18"/>
+    <mergeCell ref="C11:C18"/>
+    <mergeCell ref="D11:D18"/>
+    <mergeCell ref="E11:E18"/>
+    <mergeCell ref="F11:F18"/>
+    <mergeCell ref="B20:B27"/>
+    <mergeCell ref="C20:C27"/>
+    <mergeCell ref="D20:D27"/>
+    <mergeCell ref="E20:E27"/>
+    <mergeCell ref="F20:F27"/>
+    <mergeCell ref="B2:B9"/>
+    <mergeCell ref="C2:C9"/>
+    <mergeCell ref="D2:D9"/>
+    <mergeCell ref="E2:E9"/>
+    <mergeCell ref="F2:F9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E353E266-748B-4012-8128-88B14CF6D1CB}">
+  <dimension ref="A1:G31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="3" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="16">
+        <v>10000237</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="17">
+        <v>0</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="16">
+        <v>10029636</v>
+      </c>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="16">
+        <v>10015566</v>
+      </c>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="16">
+        <v>10003450</v>
+      </c>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="16">
+        <v>10042249</v>
+      </c>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="16">
+        <v>14000119</v>
+      </c>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="16">
+        <v>10017266</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="16">
+        <v>10017266</v>
+      </c>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="G52"/>
-    </row>
-    <row r="53" spans="1:7">
-      <c r="A53" s="2">
-        <v>10001720</v>
-      </c>
-      <c r="B53" s="12">
-        <v>445.99</v>
-      </c>
-      <c r="C53" s="12">
-        <v>36.840000000000003</v>
-      </c>
-      <c r="D53" s="12">
-        <v>409.15</v>
-      </c>
-      <c r="E53" s="12">
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="16">
+        <v>10172783</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="17">
         <v>0</v>
       </c>
-      <c r="F53" s="12">
-        <v>409.15</v>
-      </c>
-      <c r="G53" s="12" t="s">
+      <c r="F11" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="17" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
-      <c r="A54" s="2">
+    <row r="12" spans="1:7">
+      <c r="A12" s="16">
+        <v>10015566</v>
+      </c>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="16">
+        <v>10156534</v>
+      </c>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="16">
+        <v>10126399</v>
+      </c>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="16">
+        <v>10042249</v>
+      </c>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="16">
+        <v>10011399</v>
+      </c>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="16">
+        <v>10024659</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="17">
+        <v>0</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="16">
+        <v>10266745</v>
+      </c>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="16">
+        <v>10266741</v>
+      </c>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="16">
+        <v>10266744</v>
+      </c>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="16">
+        <v>14000119</v>
+      </c>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="16">
+        <v>10011118</v>
+      </c>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="16">
+        <v>10024660</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="17">
+        <v>0</v>
+      </c>
+      <c r="F25" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" s="17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="16">
+        <v>10024660</v>
+      </c>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="16">
+        <v>10022623</v>
+      </c>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="16">
+        <v>10266745</v>
+      </c>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="16">
         <v>10003450</v>
       </c>
-      <c r="B54" s="12"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
-      <c r="G54" s="12"/>
-    </row>
-    <row r="55" spans="1:7">
-      <c r="A55" s="2">
-        <v>13000295</v>
-      </c>
-      <c r="B55" s="12"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
-      <c r="G55" s="12"/>
-    </row>
-    <row r="56" spans="1:7">
-      <c r="A56" s="2">
-        <v>10005103</v>
-      </c>
-      <c r="B56" s="12"/>
-      <c r="C56" s="12"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="12"/>
-      <c r="F56" s="12"/>
-      <c r="G56" s="12"/>
-    </row>
-    <row r="57" spans="1:7">
-      <c r="A57" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G57"/>
-    </row>
-    <row r="58" spans="1:7">
-      <c r="A58" s="2">
-        <v>10011829</v>
-      </c>
-      <c r="B58" s="12">
-        <v>1742.97</v>
-      </c>
-      <c r="C58" s="12">
-        <v>48.22</v>
-      </c>
-      <c r="D58" s="12">
-        <v>1694.75</v>
-      </c>
-      <c r="E58" s="12">
-        <v>0</v>
-      </c>
-      <c r="F58" s="12">
-        <v>1694.75</v>
-      </c>
-      <c r="G58" s="12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7">
-      <c r="A59" s="2">
-        <v>10008584</v>
-      </c>
-      <c r="B59" s="12"/>
-      <c r="C59" s="12"/>
-      <c r="D59" s="12"/>
-      <c r="E59" s="12"/>
-      <c r="F59" s="12"/>
-      <c r="G59" s="12"/>
-    </row>
-    <row r="60" spans="1:7">
-      <c r="A60" s="2">
-        <v>10003450</v>
-      </c>
-      <c r="B60" s="12"/>
-      <c r="C60" s="12"/>
-      <c r="D60" s="12"/>
-      <c r="E60" s="12"/>
-      <c r="F60" s="12"/>
-      <c r="G60" s="12"/>
-    </row>
-    <row r="61" spans="1:7">
-      <c r="A61" s="2">
-        <v>10003450</v>
-      </c>
-      <c r="B61" s="12"/>
-      <c r="C61" s="12"/>
-      <c r="D61" s="12"/>
-      <c r="E61" s="12"/>
-      <c r="F61" s="12"/>
-      <c r="G61" s="12"/>
-    </row>
-    <row r="62" spans="1:7">
-      <c r="A62" s="2">
-        <v>10003450</v>
-      </c>
-      <c r="B62" s="12"/>
-      <c r="C62" s="12"/>
-      <c r="D62" s="12"/>
-      <c r="E62" s="12"/>
-      <c r="F62" s="12"/>
-      <c r="G62" s="12"/>
-    </row>
-    <row r="63" spans="1:7">
-      <c r="A63" s="2">
-        <v>13000295</v>
-      </c>
-      <c r="B63" s="12"/>
-      <c r="C63" s="12"/>
-      <c r="D63" s="12"/>
-      <c r="E63" s="12"/>
-      <c r="F63" s="12"/>
-      <c r="G63" s="12"/>
-    </row>
-    <row r="64" spans="1:7">
-      <c r="A64" s="2">
-        <v>10015188</v>
-      </c>
-      <c r="B64" s="12"/>
-      <c r="C64" s="12"/>
-      <c r="D64" s="12"/>
-      <c r="E64" s="12"/>
-      <c r="F64" s="12"/>
-      <c r="G64" s="12"/>
-    </row>
-    <row r="65" spans="1:7">
-      <c r="A65" s="2">
-        <v>10023115</v>
-      </c>
-      <c r="B65" s="12"/>
-      <c r="C65" s="12"/>
-      <c r="D65" s="12"/>
-      <c r="E65" s="12"/>
-      <c r="F65" s="12"/>
-      <c r="G65" s="12"/>
-    </row>
-    <row r="66" spans="1:7">
-      <c r="A66" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G66"/>
-    </row>
-    <row r="67" spans="1:7">
-      <c r="A67" s="2">
-        <v>10019034</v>
-      </c>
-      <c r="B67" s="12">
-        <v>847.98</v>
-      </c>
-      <c r="C67" s="12">
-        <v>73.680000000000007</v>
-      </c>
-      <c r="D67" s="12">
-        <v>774.3</v>
-      </c>
-      <c r="E67" s="12">
-        <v>0</v>
-      </c>
-      <c r="F67" s="12">
-        <v>774.3</v>
-      </c>
-      <c r="G67" s="12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7">
-      <c r="A68" s="2">
-        <v>10017013</v>
-      </c>
-      <c r="B68" s="12"/>
-      <c r="C68" s="12"/>
-      <c r="D68" s="12"/>
-      <c r="E68" s="12"/>
-      <c r="F68" s="12"/>
-      <c r="G68" s="12"/>
-    </row>
-    <row r="69" spans="1:7">
-      <c r="A69" s="2">
-        <v>10003450</v>
-      </c>
-      <c r="B69" s="12"/>
-      <c r="C69" s="12"/>
-      <c r="D69" s="12"/>
-      <c r="E69" s="12"/>
-      <c r="F69" s="12"/>
-      <c r="G69" s="12"/>
-    </row>
-    <row r="70" spans="1:7">
-      <c r="A70" s="2">
-        <v>10003450</v>
-      </c>
-      <c r="B70" s="12"/>
-      <c r="C70" s="12"/>
-      <c r="D70" s="12"/>
-      <c r="E70" s="12"/>
-      <c r="F70" s="12"/>
-      <c r="G70" s="12"/>
-    </row>
-    <row r="71" spans="1:7">
-      <c r="A71" s="2">
-        <v>13000295</v>
-      </c>
-      <c r="B71" s="12"/>
-      <c r="C71" s="12"/>
-      <c r="D71" s="12"/>
-      <c r="E71" s="12"/>
-      <c r="F71" s="12"/>
-      <c r="G71" s="12"/>
-    </row>
-    <row r="72" spans="1:7">
-      <c r="A72" s="2">
-        <v>13000295</v>
-      </c>
-      <c r="B72" s="12"/>
-      <c r="C72" s="12"/>
-      <c r="D72" s="12"/>
-      <c r="E72" s="12"/>
-      <c r="F72" s="12"/>
-      <c r="G72" s="12"/>
-    </row>
-    <row r="73" spans="1:7">
-      <c r="A73" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G73"/>
-    </row>
-    <row r="74" spans="1:7">
-      <c r="A74" s="2">
-        <v>10003450</v>
-      </c>
-      <c r="B74" s="12">
-        <v>1473.96</v>
-      </c>
-      <c r="C74" s="12">
-        <v>147.36000000000001</v>
-      </c>
-      <c r="D74" s="12">
-        <v>1326.6</v>
-      </c>
-      <c r="E74" s="12">
-        <v>0</v>
-      </c>
-      <c r="F74" s="12">
-        <v>1326.6</v>
-      </c>
-      <c r="G74" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7">
-      <c r="A75" s="2">
-        <v>10003450</v>
-      </c>
-      <c r="B75" s="12"/>
-      <c r="C75" s="12"/>
-      <c r="D75" s="12"/>
-      <c r="E75" s="12"/>
-      <c r="F75" s="12"/>
-      <c r="G75" s="12"/>
-    </row>
-    <row r="76" spans="1:7">
-      <c r="A76" s="2">
-        <v>10003450</v>
-      </c>
-      <c r="B76" s="12"/>
-      <c r="C76" s="12"/>
-      <c r="D76" s="12"/>
-      <c r="E76" s="12"/>
-      <c r="F76" s="12"/>
-      <c r="G76" s="12"/>
-    </row>
-    <row r="77" spans="1:7">
-      <c r="A77" s="2">
-        <v>10003450</v>
-      </c>
-      <c r="B77" s="12"/>
-      <c r="C77" s="12"/>
-      <c r="D77" s="12"/>
-      <c r="E77" s="12"/>
-      <c r="F77" s="12"/>
-      <c r="G77" s="12"/>
-    </row>
-    <row r="78" spans="1:7">
-      <c r="A78" s="2">
-        <v>13000295</v>
-      </c>
-      <c r="B78" s="12"/>
-      <c r="C78" s="12"/>
-      <c r="D78" s="12"/>
-      <c r="E78" s="12"/>
-      <c r="F78" s="12"/>
-      <c r="G78" s="12"/>
-    </row>
-    <row r="79" spans="1:7">
-      <c r="A79" s="2">
-        <v>13000295</v>
-      </c>
-      <c r="B79" s="12"/>
-      <c r="C79" s="12"/>
-      <c r="D79" s="12"/>
-      <c r="E79" s="12"/>
-      <c r="F79" s="12"/>
-      <c r="G79" s="12"/>
-    </row>
-    <row r="80" spans="1:7">
-      <c r="A80" s="2">
-        <v>13000295</v>
-      </c>
-      <c r="B80" s="12"/>
-      <c r="C80" s="12"/>
-      <c r="D80" s="12"/>
-      <c r="E80" s="12"/>
-      <c r="F80" s="12"/>
-      <c r="G80" s="12"/>
-    </row>
-    <row r="81" spans="1:7">
-      <c r="A81" s="2">
-        <v>13000295</v>
-      </c>
-      <c r="B81" s="12"/>
-      <c r="C81" s="12"/>
-      <c r="D81" s="12"/>
-      <c r="E81" s="12"/>
-      <c r="F81" s="12"/>
-      <c r="G81" s="12"/>
-    </row>
-    <row r="82" spans="1:7">
-      <c r="A82"/>
-      <c r="B82"/>
-      <c r="C82"/>
-      <c r="D82"/>
-      <c r="E82"/>
-      <c r="F82"/>
-      <c r="G82"/>
-    </row>
-    <row r="83" spans="1:7">
-      <c r="A83"/>
-      <c r="B83"/>
-      <c r="C83"/>
-      <c r="D83"/>
-      <c r="E83"/>
-      <c r="F83"/>
-      <c r="G83"/>
-    </row>
-    <row r="84" spans="1:7">
-      <c r="A84"/>
-      <c r="B84"/>
-      <c r="C84"/>
-      <c r="D84"/>
-      <c r="E84"/>
-      <c r="F84"/>
-      <c r="G84"/>
-    </row>
-    <row r="85" spans="1:7">
-      <c r="A85"/>
-      <c r="B85"/>
-      <c r="C85"/>
-      <c r="D85"/>
-      <c r="E85"/>
-      <c r="F85"/>
-      <c r="G85"/>
-    </row>
-    <row r="86" spans="1:7">
-      <c r="A86"/>
-      <c r="B86"/>
-      <c r="C86"/>
-      <c r="D86"/>
-      <c r="E86"/>
-      <c r="F86"/>
-      <c r="G86"/>
-    </row>
-    <row r="87" spans="1:7">
-      <c r="A87"/>
-      <c r="B87"/>
-      <c r="C87"/>
-      <c r="D87"/>
-      <c r="E87"/>
-      <c r="F87"/>
-      <c r="G87"/>
-    </row>
-    <row r="88" spans="1:7">
-      <c r="A88"/>
-      <c r="B88"/>
-      <c r="C88"/>
-      <c r="D88"/>
-      <c r="E88"/>
-      <c r="F88"/>
-      <c r="G88"/>
-    </row>
-    <row r="89" spans="1:7">
-      <c r="A89"/>
-      <c r="B89"/>
-      <c r="C89"/>
-      <c r="D89"/>
-      <c r="E89"/>
-      <c r="F89"/>
-      <c r="G89"/>
-    </row>
-    <row r="90" spans="1:7">
-      <c r="A90"/>
-      <c r="B90"/>
-      <c r="C90"/>
-      <c r="D90"/>
-      <c r="E90"/>
-      <c r="F90"/>
-      <c r="G90"/>
-    </row>
-    <row r="91" spans="1:7">
-      <c r="A91"/>
-      <c r="B91"/>
-      <c r="C91"/>
-      <c r="D91"/>
-      <c r="E91"/>
-      <c r="F91"/>
-      <c r="G91"/>
-    </row>
-    <row r="92" spans="1:7">
-      <c r="A92"/>
-      <c r="B92"/>
-      <c r="C92"/>
-      <c r="D92"/>
-      <c r="E92"/>
-      <c r="F92"/>
-      <c r="G92"/>
-    </row>
-    <row r="93" spans="1:7">
-      <c r="A93"/>
-      <c r="B93"/>
-      <c r="C93"/>
-      <c r="D93"/>
-      <c r="E93"/>
-      <c r="F93"/>
-      <c r="G93"/>
-    </row>
-    <row r="94" spans="1:7">
-      <c r="A94"/>
-      <c r="B94"/>
-      <c r="C94"/>
-      <c r="D94"/>
-      <c r="E94"/>
-      <c r="F94"/>
-      <c r="G94"/>
-    </row>
-    <row r="95" spans="1:7">
-      <c r="A95"/>
-      <c r="B95"/>
-      <c r="C95"/>
-      <c r="D95"/>
-      <c r="E95"/>
-      <c r="F95"/>
-      <c r="G95"/>
-    </row>
-    <row r="96" spans="1:7">
-      <c r="A96"/>
-      <c r="B96"/>
-      <c r="C96"/>
-      <c r="D96"/>
-      <c r="E96"/>
-      <c r="F96"/>
-      <c r="G96"/>
-    </row>
-    <row r="97" customFormat="1"/>
-    <row r="98" customFormat="1"/>
-    <row r="99" customFormat="1"/>
-    <row r="100" customFormat="1"/>
-    <row r="101" customFormat="1"/>
-    <row r="102" customFormat="1"/>
-    <row r="103" customFormat="1"/>
-    <row r="104" customFormat="1"/>
-    <row r="105" customFormat="1"/>
-    <row r="106" customFormat="1"/>
-    <row r="107" customFormat="1"/>
-    <row r="108" customFormat="1"/>
-    <row r="109" customFormat="1"/>
-    <row r="110" customFormat="1"/>
-    <row r="111" customFormat="1"/>
-    <row r="112" customFormat="1"/>
-    <row r="113" spans="1:7">
-      <c r="A113"/>
-      <c r="B113"/>
-      <c r="C113"/>
-      <c r="D113"/>
-      <c r="E113"/>
-      <c r="F113"/>
-      <c r="G113"/>
-    </row>
-    <row r="114" spans="1:7">
-      <c r="A114"/>
-      <c r="B114"/>
-      <c r="C114"/>
-      <c r="D114"/>
-      <c r="E114"/>
-      <c r="F114"/>
-      <c r="G114"/>
-    </row>
-    <row r="115" spans="1:7">
-      <c r="A115"/>
-      <c r="B115"/>
-      <c r="C115"/>
-      <c r="D115"/>
-      <c r="E115"/>
-      <c r="F115"/>
-      <c r="G115"/>
-    </row>
-    <row r="116" spans="1:7">
-      <c r="A116"/>
-      <c r="B116"/>
-      <c r="C116"/>
-      <c r="D116"/>
-      <c r="E116"/>
-      <c r="F116"/>
-      <c r="G116"/>
-    </row>
-    <row r="117" spans="1:7">
-      <c r="A117"/>
-      <c r="B117"/>
-      <c r="C117"/>
-      <c r="D117"/>
-      <c r="E117"/>
-      <c r="F117"/>
-      <c r="G117"/>
-    </row>
-    <row r="118" spans="1:7">
-      <c r="A118"/>
-      <c r="B118"/>
-      <c r="C118"/>
-      <c r="D118"/>
-      <c r="E118"/>
-      <c r="F118"/>
-      <c r="G118"/>
-    </row>
-    <row r="119" spans="1:7">
-      <c r="A119"/>
-      <c r="B119"/>
-      <c r="C119"/>
-      <c r="D119"/>
-      <c r="E119"/>
-      <c r="F119"/>
-      <c r="G119"/>
-    </row>
-    <row r="120" spans="1:7">
-      <c r="A120"/>
-      <c r="B120"/>
-      <c r="C120"/>
-      <c r="D120"/>
-      <c r="E120"/>
-      <c r="F120"/>
-      <c r="G120"/>
-    </row>
-    <row r="121" spans="1:7">
-      <c r="G121"/>
-    </row>
-    <row r="122" spans="1:7">
-      <c r="G122"/>
-    </row>
-    <row r="123" spans="1:7">
-      <c r="G123"/>
-    </row>
-    <row r="124" spans="1:7">
-      <c r="G124"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="16">
+        <v>10011404</v>
+      </c>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="16">
+        <v>10011402</v>
+      </c>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="72">
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="C2:C6"/>
-    <mergeCell ref="D2:D6"/>
-    <mergeCell ref="E2:E6"/>
-    <mergeCell ref="F2:F6"/>
-    <mergeCell ref="B17:B24"/>
-    <mergeCell ref="C17:C24"/>
-    <mergeCell ref="D17:D24"/>
-    <mergeCell ref="E17:E24"/>
-    <mergeCell ref="F17:F24"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="F12:F15"/>
-    <mergeCell ref="B35:B42"/>
-    <mergeCell ref="C35:C42"/>
-    <mergeCell ref="D35:D42"/>
-    <mergeCell ref="E35:E42"/>
-    <mergeCell ref="F35:F42"/>
-    <mergeCell ref="B26:B33"/>
-    <mergeCell ref="C26:C33"/>
-    <mergeCell ref="D26:D33"/>
-    <mergeCell ref="E26:E33"/>
-    <mergeCell ref="F26:F33"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="C49:C51"/>
-    <mergeCell ref="D49:D51"/>
-    <mergeCell ref="E49:E51"/>
-    <mergeCell ref="F49:F51"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="C44:C47"/>
-    <mergeCell ref="D44:D47"/>
-    <mergeCell ref="E44:E47"/>
-    <mergeCell ref="F44:F47"/>
-    <mergeCell ref="B58:B65"/>
-    <mergeCell ref="C58:C65"/>
-    <mergeCell ref="D58:D65"/>
-    <mergeCell ref="E58:E65"/>
-    <mergeCell ref="F58:F65"/>
-    <mergeCell ref="B74:B81"/>
-    <mergeCell ref="C74:C81"/>
-    <mergeCell ref="D74:D81"/>
-    <mergeCell ref="E74:E81"/>
-    <mergeCell ref="F74:F81"/>
-    <mergeCell ref="B67:B72"/>
-    <mergeCell ref="C67:C72"/>
-    <mergeCell ref="D67:D72"/>
-    <mergeCell ref="E67:E72"/>
-    <mergeCell ref="F67:F72"/>
-    <mergeCell ref="F53:F56"/>
-    <mergeCell ref="E53:E56"/>
-    <mergeCell ref="D53:D56"/>
-    <mergeCell ref="C53:C56"/>
-    <mergeCell ref="B53:B56"/>
-    <mergeCell ref="G2:G6"/>
-    <mergeCell ref="G74:G81"/>
-    <mergeCell ref="G67:G72"/>
-    <mergeCell ref="G58:G65"/>
-    <mergeCell ref="G53:G56"/>
-    <mergeCell ref="G49:G51"/>
-    <mergeCell ref="G44:G47"/>
-    <mergeCell ref="G35:G42"/>
-    <mergeCell ref="G26:G33"/>
-    <mergeCell ref="G17:G24"/>
-    <mergeCell ref="G12:G15"/>
-    <mergeCell ref="G8:G10"/>
+  <mergeCells count="24">
+    <mergeCell ref="B25:B31"/>
+    <mergeCell ref="C25:C31"/>
+    <mergeCell ref="D25:D31"/>
+    <mergeCell ref="E25:E31"/>
+    <mergeCell ref="F25:F31"/>
+    <mergeCell ref="G25:G31"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="C18:C23"/>
+    <mergeCell ref="D18:D23"/>
+    <mergeCell ref="E18:E23"/>
+    <mergeCell ref="F18:F23"/>
+    <mergeCell ref="G18:G23"/>
+    <mergeCell ref="B11:B16"/>
+    <mergeCell ref="C11:C16"/>
+    <mergeCell ref="D11:D16"/>
+    <mergeCell ref="E11:E16"/>
+    <mergeCell ref="F11:F16"/>
+    <mergeCell ref="G11:G16"/>
+    <mergeCell ref="B2:B9"/>
+    <mergeCell ref="C2:C9"/>
+    <mergeCell ref="D2:D9"/>
+    <mergeCell ref="E2:E9"/>
+    <mergeCell ref="F2:F9"/>
+    <mergeCell ref="G2:G9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2869,14 +2733,6 @@
     <row r="68" customFormat="1"/>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="D19:D26"/>
-    <mergeCell ref="E19:E26"/>
-    <mergeCell ref="F19:F26"/>
-    <mergeCell ref="B28:B33"/>
-    <mergeCell ref="C28:C33"/>
-    <mergeCell ref="D28:D33"/>
-    <mergeCell ref="E28:E33"/>
-    <mergeCell ref="F28:F33"/>
     <mergeCell ref="G19:G26"/>
     <mergeCell ref="G28:G33"/>
     <mergeCell ref="G2:G8"/>
@@ -2893,6 +2749,14 @@
     <mergeCell ref="F10:F17"/>
     <mergeCell ref="B19:B26"/>
     <mergeCell ref="C19:C26"/>
+    <mergeCell ref="D19:D26"/>
+    <mergeCell ref="E19:E26"/>
+    <mergeCell ref="F19:F26"/>
+    <mergeCell ref="B28:B33"/>
+    <mergeCell ref="C28:C33"/>
+    <mergeCell ref="D28:D33"/>
+    <mergeCell ref="E28:E33"/>
+    <mergeCell ref="F28:F33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3802,39 +3666,11 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="B66:B73"/>
-    <mergeCell ref="C66:C73"/>
-    <mergeCell ref="D66:D73"/>
-    <mergeCell ref="E66:E73"/>
-    <mergeCell ref="F66:F73"/>
-    <mergeCell ref="B58:B64"/>
-    <mergeCell ref="C58:C64"/>
-    <mergeCell ref="D58:D64"/>
-    <mergeCell ref="E58:E64"/>
-    <mergeCell ref="F58:F64"/>
-    <mergeCell ref="B50:B56"/>
-    <mergeCell ref="C50:C56"/>
-    <mergeCell ref="D50:D56"/>
-    <mergeCell ref="E50:E56"/>
-    <mergeCell ref="F50:F56"/>
-    <mergeCell ref="B41:B48"/>
-    <mergeCell ref="C41:C48"/>
-    <mergeCell ref="D41:D48"/>
-    <mergeCell ref="E41:E48"/>
-    <mergeCell ref="F41:F48"/>
-    <mergeCell ref="B34:B39"/>
-    <mergeCell ref="C34:C39"/>
-    <mergeCell ref="D34:D39"/>
-    <mergeCell ref="E34:E39"/>
-    <mergeCell ref="F34:F39"/>
-    <mergeCell ref="D18:D23"/>
-    <mergeCell ref="E18:E23"/>
-    <mergeCell ref="F18:F23"/>
-    <mergeCell ref="B25:B32"/>
-    <mergeCell ref="C25:C32"/>
-    <mergeCell ref="D25:D32"/>
-    <mergeCell ref="E25:E32"/>
-    <mergeCell ref="F25:F32"/>
+    <mergeCell ref="G18:G23"/>
+    <mergeCell ref="G11:G16"/>
+    <mergeCell ref="G2:G9"/>
+    <mergeCell ref="G50:G56"/>
+    <mergeCell ref="G58:G64"/>
     <mergeCell ref="G66:G73"/>
     <mergeCell ref="G25:G32"/>
     <mergeCell ref="G34:G39"/>
@@ -3851,11 +3687,39 @@
     <mergeCell ref="F11:F16"/>
     <mergeCell ref="B18:B23"/>
     <mergeCell ref="C18:C23"/>
-    <mergeCell ref="G18:G23"/>
-    <mergeCell ref="G11:G16"/>
-    <mergeCell ref="G2:G9"/>
-    <mergeCell ref="G50:G56"/>
-    <mergeCell ref="G58:G64"/>
+    <mergeCell ref="D18:D23"/>
+    <mergeCell ref="E18:E23"/>
+    <mergeCell ref="F18:F23"/>
+    <mergeCell ref="B25:B32"/>
+    <mergeCell ref="C25:C32"/>
+    <mergeCell ref="D25:D32"/>
+    <mergeCell ref="E25:E32"/>
+    <mergeCell ref="F25:F32"/>
+    <mergeCell ref="B34:B39"/>
+    <mergeCell ref="C34:C39"/>
+    <mergeCell ref="D34:D39"/>
+    <mergeCell ref="E34:E39"/>
+    <mergeCell ref="F34:F39"/>
+    <mergeCell ref="B41:B48"/>
+    <mergeCell ref="C41:C48"/>
+    <mergeCell ref="D41:D48"/>
+    <mergeCell ref="E41:E48"/>
+    <mergeCell ref="F41:F48"/>
+    <mergeCell ref="B50:B56"/>
+    <mergeCell ref="C50:C56"/>
+    <mergeCell ref="D50:D56"/>
+    <mergeCell ref="E50:E56"/>
+    <mergeCell ref="F50:F56"/>
+    <mergeCell ref="B58:B64"/>
+    <mergeCell ref="C58:C64"/>
+    <mergeCell ref="D58:D64"/>
+    <mergeCell ref="E58:E64"/>
+    <mergeCell ref="F58:F64"/>
+    <mergeCell ref="B66:B73"/>
+    <mergeCell ref="C66:C73"/>
+    <mergeCell ref="D66:D73"/>
+    <mergeCell ref="E66:E73"/>
+    <mergeCell ref="F66:F73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4444,36 +4308,36 @@
     <row r="50" customFormat="1"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="G27:G33"/>
+    <mergeCell ref="G35:G41"/>
+    <mergeCell ref="G2:G9"/>
+    <mergeCell ref="G11:G16"/>
+    <mergeCell ref="G18:G25"/>
+    <mergeCell ref="B2:B9"/>
+    <mergeCell ref="C2:C9"/>
+    <mergeCell ref="D2:D9"/>
+    <mergeCell ref="E2:E9"/>
+    <mergeCell ref="F2:F9"/>
+    <mergeCell ref="B11:B16"/>
+    <mergeCell ref="C11:C16"/>
+    <mergeCell ref="D11:D16"/>
+    <mergeCell ref="E11:E16"/>
+    <mergeCell ref="F11:F16"/>
+    <mergeCell ref="B18:B25"/>
+    <mergeCell ref="C18:C25"/>
+    <mergeCell ref="D18:D25"/>
+    <mergeCell ref="E18:E25"/>
+    <mergeCell ref="F18:F25"/>
+    <mergeCell ref="B27:B33"/>
+    <mergeCell ref="C27:C33"/>
+    <mergeCell ref="D27:D33"/>
+    <mergeCell ref="E27:E33"/>
+    <mergeCell ref="F27:F33"/>
     <mergeCell ref="B35:B41"/>
     <mergeCell ref="C35:C41"/>
     <mergeCell ref="D35:D41"/>
     <mergeCell ref="E35:E41"/>
     <mergeCell ref="F35:F41"/>
-    <mergeCell ref="B27:B33"/>
-    <mergeCell ref="C27:C33"/>
-    <mergeCell ref="D27:D33"/>
-    <mergeCell ref="E27:E33"/>
-    <mergeCell ref="F27:F33"/>
-    <mergeCell ref="B18:B25"/>
-    <mergeCell ref="C18:C25"/>
-    <mergeCell ref="D18:D25"/>
-    <mergeCell ref="E18:E25"/>
-    <mergeCell ref="F18:F25"/>
-    <mergeCell ref="B11:B16"/>
-    <mergeCell ref="C11:C16"/>
-    <mergeCell ref="D11:D16"/>
-    <mergeCell ref="E11:E16"/>
-    <mergeCell ref="F11:F16"/>
-    <mergeCell ref="B2:B9"/>
-    <mergeCell ref="C2:C9"/>
-    <mergeCell ref="D2:D9"/>
-    <mergeCell ref="E2:E9"/>
-    <mergeCell ref="F2:F9"/>
-    <mergeCell ref="G27:G33"/>
-    <mergeCell ref="G35:G41"/>
-    <mergeCell ref="G2:G9"/>
-    <mergeCell ref="G11:G16"/>
-    <mergeCell ref="G18:G25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5283,31 +5147,11 @@
     <row r="84" customFormat="1"/>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="B52:B59"/>
-    <mergeCell ref="C52:C59"/>
-    <mergeCell ref="D52:D59"/>
-    <mergeCell ref="E52:E59"/>
-    <mergeCell ref="F52:F59"/>
-    <mergeCell ref="B45:B50"/>
-    <mergeCell ref="C45:C50"/>
-    <mergeCell ref="D45:D50"/>
-    <mergeCell ref="E45:E50"/>
-    <mergeCell ref="F45:F50"/>
-    <mergeCell ref="B36:B43"/>
-    <mergeCell ref="C36:C43"/>
-    <mergeCell ref="D36:D43"/>
-    <mergeCell ref="E36:E43"/>
-    <mergeCell ref="F36:F43"/>
-    <mergeCell ref="B29:B34"/>
-    <mergeCell ref="C29:C34"/>
-    <mergeCell ref="D29:D34"/>
-    <mergeCell ref="E29:E34"/>
-    <mergeCell ref="F29:F34"/>
-    <mergeCell ref="B20:B27"/>
-    <mergeCell ref="C20:C27"/>
-    <mergeCell ref="D20:D27"/>
-    <mergeCell ref="E20:E27"/>
-    <mergeCell ref="F20:F27"/>
+    <mergeCell ref="G36:G43"/>
+    <mergeCell ref="G45:G50"/>
+    <mergeCell ref="G52:G59"/>
+    <mergeCell ref="G20:G27"/>
+    <mergeCell ref="G29:G34"/>
     <mergeCell ref="G2:G9"/>
     <mergeCell ref="G11:G18"/>
     <mergeCell ref="B2:B9"/>
@@ -5320,11 +5164,31 @@
     <mergeCell ref="D11:D18"/>
     <mergeCell ref="E11:E18"/>
     <mergeCell ref="F11:F18"/>
-    <mergeCell ref="G36:G43"/>
-    <mergeCell ref="G45:G50"/>
-    <mergeCell ref="G52:G59"/>
-    <mergeCell ref="G20:G27"/>
-    <mergeCell ref="G29:G34"/>
+    <mergeCell ref="B20:B27"/>
+    <mergeCell ref="C20:C27"/>
+    <mergeCell ref="D20:D27"/>
+    <mergeCell ref="E20:E27"/>
+    <mergeCell ref="F20:F27"/>
+    <mergeCell ref="B29:B34"/>
+    <mergeCell ref="C29:C34"/>
+    <mergeCell ref="D29:D34"/>
+    <mergeCell ref="E29:E34"/>
+    <mergeCell ref="F29:F34"/>
+    <mergeCell ref="B36:B43"/>
+    <mergeCell ref="C36:C43"/>
+    <mergeCell ref="D36:D43"/>
+    <mergeCell ref="E36:E43"/>
+    <mergeCell ref="F36:F43"/>
+    <mergeCell ref="B45:B50"/>
+    <mergeCell ref="C45:C50"/>
+    <mergeCell ref="D45:D50"/>
+    <mergeCell ref="E45:E50"/>
+    <mergeCell ref="F45:F50"/>
+    <mergeCell ref="B52:B59"/>
+    <mergeCell ref="C52:C59"/>
+    <mergeCell ref="D52:D59"/>
+    <mergeCell ref="E52:E59"/>
+    <mergeCell ref="F52:F59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5939,42 +5803,42 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="B35:B40"/>
-    <mergeCell ref="C35:C40"/>
-    <mergeCell ref="D35:D40"/>
-    <mergeCell ref="E35:E40"/>
-    <mergeCell ref="F35:F40"/>
-    <mergeCell ref="B42:B48"/>
-    <mergeCell ref="C42:C48"/>
-    <mergeCell ref="D42:D48"/>
-    <mergeCell ref="E42:E48"/>
-    <mergeCell ref="F42:F48"/>
-    <mergeCell ref="B27:B33"/>
-    <mergeCell ref="C27:C33"/>
-    <mergeCell ref="D27:D33"/>
-    <mergeCell ref="E27:E33"/>
-    <mergeCell ref="F27:F33"/>
-    <mergeCell ref="B11:B16"/>
-    <mergeCell ref="C11:C16"/>
-    <mergeCell ref="D11:D16"/>
-    <mergeCell ref="E11:E16"/>
-    <mergeCell ref="F11:F16"/>
-    <mergeCell ref="B18:B25"/>
-    <mergeCell ref="C18:C25"/>
-    <mergeCell ref="D18:D25"/>
-    <mergeCell ref="E18:E25"/>
-    <mergeCell ref="F18:F25"/>
-    <mergeCell ref="B2:B9"/>
-    <mergeCell ref="C2:C9"/>
-    <mergeCell ref="D2:D9"/>
-    <mergeCell ref="E2:E9"/>
-    <mergeCell ref="F2:F9"/>
     <mergeCell ref="G27:G33"/>
     <mergeCell ref="G35:G40"/>
     <mergeCell ref="G42:G48"/>
     <mergeCell ref="G2:G9"/>
     <mergeCell ref="G11:G16"/>
     <mergeCell ref="G18:G25"/>
+    <mergeCell ref="B2:B9"/>
+    <mergeCell ref="C2:C9"/>
+    <mergeCell ref="D2:D9"/>
+    <mergeCell ref="E2:E9"/>
+    <mergeCell ref="F2:F9"/>
+    <mergeCell ref="B18:B25"/>
+    <mergeCell ref="C18:C25"/>
+    <mergeCell ref="D18:D25"/>
+    <mergeCell ref="E18:E25"/>
+    <mergeCell ref="F18:F25"/>
+    <mergeCell ref="B11:B16"/>
+    <mergeCell ref="C11:C16"/>
+    <mergeCell ref="D11:D16"/>
+    <mergeCell ref="E11:E16"/>
+    <mergeCell ref="F11:F16"/>
+    <mergeCell ref="B27:B33"/>
+    <mergeCell ref="C27:C33"/>
+    <mergeCell ref="D27:D33"/>
+    <mergeCell ref="E27:E33"/>
+    <mergeCell ref="F27:F33"/>
+    <mergeCell ref="B42:B48"/>
+    <mergeCell ref="C42:C48"/>
+    <mergeCell ref="D42:D48"/>
+    <mergeCell ref="E42:E48"/>
+    <mergeCell ref="F42:F48"/>
+    <mergeCell ref="B35:B40"/>
+    <mergeCell ref="C35:C40"/>
+    <mergeCell ref="D35:D40"/>
+    <mergeCell ref="E35:E40"/>
+    <mergeCell ref="F35:F40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6906,36 +6770,14 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="B68:B75"/>
-    <mergeCell ref="C68:C75"/>
-    <mergeCell ref="D68:D75"/>
-    <mergeCell ref="E68:E75"/>
-    <mergeCell ref="F68:F75"/>
-    <mergeCell ref="B60:B66"/>
-    <mergeCell ref="C60:C66"/>
-    <mergeCell ref="D60:D66"/>
-    <mergeCell ref="E60:E66"/>
-    <mergeCell ref="F60:F66"/>
-    <mergeCell ref="B52:B58"/>
-    <mergeCell ref="C52:C58"/>
-    <mergeCell ref="D52:D58"/>
-    <mergeCell ref="E52:E58"/>
-    <mergeCell ref="F52:F58"/>
-    <mergeCell ref="B45:B50"/>
-    <mergeCell ref="C45:C50"/>
-    <mergeCell ref="D45:D50"/>
-    <mergeCell ref="E45:E50"/>
-    <mergeCell ref="F45:F50"/>
-    <mergeCell ref="B38:B43"/>
-    <mergeCell ref="C38:C43"/>
-    <mergeCell ref="D38:D43"/>
-    <mergeCell ref="E38:E43"/>
-    <mergeCell ref="F38:F43"/>
-    <mergeCell ref="B29:B36"/>
-    <mergeCell ref="C29:C36"/>
-    <mergeCell ref="D29:D36"/>
-    <mergeCell ref="E29:E36"/>
-    <mergeCell ref="F29:F36"/>
+    <mergeCell ref="E11:E18"/>
+    <mergeCell ref="F11:F18"/>
+    <mergeCell ref="G52:G58"/>
+    <mergeCell ref="G60:G66"/>
+    <mergeCell ref="G68:G75"/>
+    <mergeCell ref="G29:G36"/>
+    <mergeCell ref="G38:G43"/>
+    <mergeCell ref="G45:G50"/>
     <mergeCell ref="G2:G9"/>
     <mergeCell ref="G20:G27"/>
     <mergeCell ref="B2:B9"/>
@@ -6952,14 +6794,36 @@
     <mergeCell ref="B11:B18"/>
     <mergeCell ref="C11:C18"/>
     <mergeCell ref="D11:D18"/>
-    <mergeCell ref="E11:E18"/>
-    <mergeCell ref="F11:F18"/>
-    <mergeCell ref="G52:G58"/>
-    <mergeCell ref="G60:G66"/>
-    <mergeCell ref="G68:G75"/>
-    <mergeCell ref="G29:G36"/>
-    <mergeCell ref="G38:G43"/>
-    <mergeCell ref="G45:G50"/>
+    <mergeCell ref="B29:B36"/>
+    <mergeCell ref="C29:C36"/>
+    <mergeCell ref="D29:D36"/>
+    <mergeCell ref="E29:E36"/>
+    <mergeCell ref="F29:F36"/>
+    <mergeCell ref="B38:B43"/>
+    <mergeCell ref="C38:C43"/>
+    <mergeCell ref="D38:D43"/>
+    <mergeCell ref="E38:E43"/>
+    <mergeCell ref="F38:F43"/>
+    <mergeCell ref="B45:B50"/>
+    <mergeCell ref="C45:C50"/>
+    <mergeCell ref="D45:D50"/>
+    <mergeCell ref="E45:E50"/>
+    <mergeCell ref="F45:F50"/>
+    <mergeCell ref="B52:B58"/>
+    <mergeCell ref="C52:C58"/>
+    <mergeCell ref="D52:D58"/>
+    <mergeCell ref="E52:E58"/>
+    <mergeCell ref="F52:F58"/>
+    <mergeCell ref="B60:B66"/>
+    <mergeCell ref="C60:C66"/>
+    <mergeCell ref="D60:D66"/>
+    <mergeCell ref="E60:E66"/>
+    <mergeCell ref="F60:F66"/>
+    <mergeCell ref="B68:B75"/>
+    <mergeCell ref="C68:C75"/>
+    <mergeCell ref="D68:D75"/>
+    <mergeCell ref="E68:E75"/>
+    <mergeCell ref="F68:F75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7014,10 +6878,10 @@
       <c r="B2" s="12">
         <v>344</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="13">
         <v>20</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="13">
         <v>324</v>
       </c>
       <c r="E2" s="12">
@@ -7035,8 +6899,8 @@
         <v>11000392</v>
       </c>
       <c r="B3" s="12"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
@@ -7046,8 +6910,8 @@
         <v>11000392</v>
       </c>
       <c r="B4" s="12"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -7057,8 +6921,8 @@
         <v>11000392</v>
       </c>
       <c r="B5" s="12"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
@@ -7068,8 +6932,8 @@
         <v>10042249</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -7079,8 +6943,8 @@
         <v>10042249</v>
       </c>
       <c r="B7" s="12"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
@@ -7090,8 +6954,8 @@
         <v>10042249</v>
       </c>
       <c r="B8" s="12"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
@@ -7101,8 +6965,8 @@
         <v>10042249</v>
       </c>
       <c r="B9" s="12"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
@@ -7125,10 +6989,10 @@
       <c r="B11" s="12">
         <v>254.75</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="14">
         <v>20.6</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="14">
         <v>234.15</v>
       </c>
       <c r="E11" s="12">
@@ -7146,8 +7010,8 @@
         <v>10029636</v>
       </c>
       <c r="B12" s="12"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
@@ -7157,8 +7021,8 @@
         <v>11000392</v>
       </c>
       <c r="B13" s="12"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
@@ -7168,8 +7032,8 @@
         <v>11000392</v>
       </c>
       <c r="B14" s="12"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
@@ -7179,8 +7043,8 @@
         <v>11000392</v>
       </c>
       <c r="B15" s="12"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
@@ -7190,8 +7054,8 @@
         <v>11000392</v>
       </c>
       <c r="B16" s="12"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
@@ -7201,8 +7065,8 @@
         <v>10042249</v>
       </c>
       <c r="B17" s="12"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
@@ -7212,8 +7076,8 @@
         <v>10042249</v>
       </c>
       <c r="B18" s="12"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
@@ -7223,8 +7087,8 @@
         <v>10042249</v>
       </c>
       <c r="B19" s="12"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
@@ -8436,12 +8300,42 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="G2:G9"/>
-    <mergeCell ref="B2:B9"/>
-    <mergeCell ref="C2:C9"/>
-    <mergeCell ref="D2:D9"/>
-    <mergeCell ref="E2:E9"/>
-    <mergeCell ref="F2:F9"/>
+    <mergeCell ref="G82:G90"/>
+    <mergeCell ref="B73:B80"/>
+    <mergeCell ref="C73:C80"/>
+    <mergeCell ref="D73:D80"/>
+    <mergeCell ref="E73:E80"/>
+    <mergeCell ref="F73:F80"/>
+    <mergeCell ref="G73:G80"/>
+    <mergeCell ref="B82:B90"/>
+    <mergeCell ref="C82:C90"/>
+    <mergeCell ref="D82:D90"/>
+    <mergeCell ref="E82:E90"/>
+    <mergeCell ref="F82:F90"/>
+    <mergeCell ref="G62:G71"/>
+    <mergeCell ref="B51:B60"/>
+    <mergeCell ref="C51:C60"/>
+    <mergeCell ref="D51:D60"/>
+    <mergeCell ref="E51:E60"/>
+    <mergeCell ref="F51:F60"/>
+    <mergeCell ref="G51:G60"/>
+    <mergeCell ref="B62:B71"/>
+    <mergeCell ref="C62:C71"/>
+    <mergeCell ref="D62:D71"/>
+    <mergeCell ref="E62:E71"/>
+    <mergeCell ref="F62:F71"/>
+    <mergeCell ref="G40:G49"/>
+    <mergeCell ref="B31:B38"/>
+    <mergeCell ref="C31:C38"/>
+    <mergeCell ref="D31:D38"/>
+    <mergeCell ref="E31:E38"/>
+    <mergeCell ref="F31:F38"/>
+    <mergeCell ref="G31:G38"/>
+    <mergeCell ref="B40:B49"/>
+    <mergeCell ref="C40:C49"/>
+    <mergeCell ref="D40:D49"/>
+    <mergeCell ref="E40:E49"/>
+    <mergeCell ref="F40:F49"/>
     <mergeCell ref="G21:G29"/>
     <mergeCell ref="B11:B19"/>
     <mergeCell ref="C11:C19"/>
@@ -8454,53 +8348,23 @@
     <mergeCell ref="D21:D29"/>
     <mergeCell ref="E21:E29"/>
     <mergeCell ref="F21:F29"/>
-    <mergeCell ref="G40:G49"/>
-    <mergeCell ref="B31:B38"/>
-    <mergeCell ref="C31:C38"/>
-    <mergeCell ref="D31:D38"/>
-    <mergeCell ref="E31:E38"/>
-    <mergeCell ref="F31:F38"/>
-    <mergeCell ref="G31:G38"/>
-    <mergeCell ref="B40:B49"/>
-    <mergeCell ref="C40:C49"/>
-    <mergeCell ref="D40:D49"/>
-    <mergeCell ref="E40:E49"/>
-    <mergeCell ref="F40:F49"/>
-    <mergeCell ref="G62:G71"/>
-    <mergeCell ref="B51:B60"/>
-    <mergeCell ref="C51:C60"/>
-    <mergeCell ref="D51:D60"/>
-    <mergeCell ref="E51:E60"/>
-    <mergeCell ref="F51:F60"/>
-    <mergeCell ref="G51:G60"/>
-    <mergeCell ref="B62:B71"/>
-    <mergeCell ref="C62:C71"/>
-    <mergeCell ref="D62:D71"/>
-    <mergeCell ref="E62:E71"/>
-    <mergeCell ref="F62:F71"/>
-    <mergeCell ref="G82:G90"/>
-    <mergeCell ref="B73:B80"/>
-    <mergeCell ref="C73:C80"/>
-    <mergeCell ref="D73:D80"/>
-    <mergeCell ref="E73:E80"/>
-    <mergeCell ref="F73:F80"/>
-    <mergeCell ref="G73:G80"/>
-    <mergeCell ref="B82:B90"/>
-    <mergeCell ref="C82:C90"/>
-    <mergeCell ref="D82:D90"/>
-    <mergeCell ref="E82:E90"/>
-    <mergeCell ref="F82:F90"/>
+    <mergeCell ref="G2:G9"/>
+    <mergeCell ref="B2:B9"/>
+    <mergeCell ref="C2:C9"/>
+    <mergeCell ref="D2:D9"/>
+    <mergeCell ref="E2:E9"/>
+    <mergeCell ref="F2:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6A820D7-2A77-47D5-9EF4-EA2F91DD3F2E}">
-  <dimension ref="A1:G52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32994263-25BE-40BB-935D-F1983009F224}">
+  <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44:B51"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49:F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -8538,148 +8402,160 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="2">
-        <v>10029055</v>
+      <c r="A2" s="7">
+        <v>10023698</v>
       </c>
       <c r="B2" s="12">
-        <v>399.5</v>
-      </c>
-      <c r="C2" s="12">
-        <v>33.5</v>
-      </c>
-      <c r="D2" s="12">
-        <v>366</v>
+        <v>394.99</v>
+      </c>
+      <c r="C2" s="13">
+        <v>36.840000000000003</v>
+      </c>
+      <c r="D2" s="13">
+        <v>358.15</v>
       </c>
       <c r="E2" s="12">
         <v>0</v>
       </c>
       <c r="F2" s="12">
-        <v>366</v>
+        <v>358.15</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="2">
-        <v>10016979</v>
+      <c r="A3" s="7">
+        <v>10018762</v>
       </c>
       <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="2">
-        <v>10016981</v>
+      <c r="A4" s="7">
+        <v>10003482</v>
       </c>
       <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="2">
-        <v>10017022</v>
+      <c r="A5" s="7">
+        <v>10003450</v>
       </c>
       <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="2">
-        <v>10029636</v>
+      <c r="A6" s="7">
+        <v>13000295</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="2">
-        <v>10029636</v>
-      </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="2">
-        <v>10033046</v>
-      </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="2">
-        <v>10017090</v>
+    <row r="7" spans="1:7" ht="15.6">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.6">
+      <c r="A8" s="6">
+        <v>10018762</v>
+      </c>
+      <c r="B8" s="12">
+        <v>326.5</v>
+      </c>
+      <c r="C8" s="14">
+        <v>31.15</v>
+      </c>
+      <c r="D8" s="14">
+        <v>295.35000000000002</v>
+      </c>
+      <c r="E8" s="12">
+        <v>34.9</v>
+      </c>
+      <c r="F8" s="12">
+        <v>330.25</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.6">
+      <c r="A9" s="6">
+        <v>10015790</v>
       </c>
       <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
     </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:7" ht="15.6">
+      <c r="A10" s="6">
+        <v>13000295</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G10"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="2">
-        <v>10031016</v>
-      </c>
-      <c r="B11" s="12">
-        <v>228.5</v>
-      </c>
-      <c r="C11" s="12">
-        <v>33.5</v>
-      </c>
-      <c r="D11" s="12">
-        <v>195</v>
-      </c>
-      <c r="E11" s="12">
-        <v>34.9</v>
-      </c>
-      <c r="F11" s="12">
-        <v>229.9</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>7</v>
-      </c>
+      <c r="G11"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="2">
-        <v>10029055</v>
-      </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
+        <v>10003480</v>
+      </c>
+      <c r="B12" s="12">
+        <v>434.49</v>
+      </c>
+      <c r="C12" s="12">
+        <v>36.840000000000003</v>
+      </c>
+      <c r="D12" s="12">
+        <v>397.65</v>
+      </c>
+      <c r="E12" s="12">
+        <v>0</v>
+      </c>
+      <c r="F12" s="12">
+        <v>397.65</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="2">
-        <v>10029055</v>
+        <v>10017642</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
@@ -8690,7 +8566,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="2">
-        <v>10005052</v>
+        <v>10003450</v>
       </c>
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
@@ -8701,7 +8577,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="2">
-        <v>10005052</v>
+        <v>13000295</v>
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
@@ -8711,30 +8587,37 @@
       <c r="G15" s="12"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="2">
-        <v>10014863</v>
-      </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
+      <c r="A16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="2">
-        <v>10029636</v>
-      </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
+        <v>10015247</v>
+      </c>
+      <c r="B17" s="12">
+        <v>897.48</v>
+      </c>
+      <c r="C17" s="12">
+        <v>73.680000000000007</v>
+      </c>
+      <c r="D17" s="12">
+        <v>823.8</v>
+      </c>
+      <c r="E17" s="12">
+        <v>0</v>
+      </c>
+      <c r="F17" s="12">
+        <v>823.8</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="2">
-        <v>10029636</v>
+        <v>10017003</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -8744,37 +8627,30 @@
       <c r="G18" s="12"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G19"/>
+      <c r="A19" s="2">
+        <v>10003450</v>
+      </c>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="2">
-        <v>10006676</v>
-      </c>
-      <c r="B20" s="12">
-        <v>217.75</v>
-      </c>
-      <c r="C20" s="12">
-        <v>16.75</v>
-      </c>
-      <c r="D20" s="12">
-        <v>201</v>
-      </c>
-      <c r="E20" s="12">
-        <v>0</v>
-      </c>
-      <c r="F20" s="12">
-        <v>201</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>9</v>
-      </c>
+        <v>10003450</v>
+      </c>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="2">
-        <v>10005104</v>
+        <v>13000295</v>
       </c>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
@@ -8785,7 +8661,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="2">
-        <v>10029052</v>
+        <v>13000295</v>
       </c>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
@@ -8796,7 +8672,7 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="2">
-        <v>10005052</v>
+        <v>10023194</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
@@ -8807,7 +8683,7 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="2">
-        <v>10022377</v>
+        <v>10023190</v>
       </c>
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
@@ -8817,30 +8693,37 @@
       <c r="G24" s="12"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="2">
-        <v>10014863</v>
-      </c>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
+      <c r="A25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25"/>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="2">
-        <v>10029636</v>
-      </c>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
+        <v>10015790</v>
+      </c>
+      <c r="B26" s="12">
+        <v>614.98</v>
+      </c>
+      <c r="C26" s="12">
+        <v>42.53</v>
+      </c>
+      <c r="D26" s="12">
+        <v>572.45000000000005</v>
+      </c>
+      <c r="E26" s="12">
+        <v>0</v>
+      </c>
+      <c r="F26" s="12">
+        <v>572.45000000000005</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="2">
-        <v>10008866</v>
+        <v>10014865</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
@@ -8850,37 +8733,30 @@
       <c r="G27" s="12"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G28"/>
+      <c r="A28" s="2">
+        <v>10028562</v>
+      </c>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="2">
-        <v>10021661</v>
-      </c>
-      <c r="B29" s="12">
-        <v>1707</v>
-      </c>
-      <c r="C29" s="12">
-        <v>33.5</v>
-      </c>
-      <c r="D29" s="12">
-        <v>1673.5</v>
-      </c>
-      <c r="E29" s="12">
-        <v>0</v>
-      </c>
-      <c r="F29" s="12">
-        <v>1673.5</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>7</v>
-      </c>
+        <v>10004378</v>
+      </c>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="2">
-        <v>10002298</v>
+        <v>10003450</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
@@ -8891,7 +8767,7 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="2">
-        <v>10029636</v>
+        <v>10003450</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
@@ -8902,7 +8778,7 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="2">
-        <v>10029636</v>
+        <v>13000295</v>
       </c>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
@@ -8913,7 +8789,7 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="2">
-        <v>10001399</v>
+        <v>10015188</v>
       </c>
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
@@ -8923,59 +8799,59 @@
       <c r="G33" s="12"/>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="2">
-        <v>10019602</v>
-      </c>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
+      <c r="A34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34"/>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="2">
-        <v>10003352</v>
-      </c>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
+        <v>10028783</v>
+      </c>
+      <c r="B35" s="12">
+        <v>1451.48</v>
+      </c>
+      <c r="C35" s="12">
+        <v>104.83</v>
+      </c>
+      <c r="D35" s="12">
+        <v>1346.65</v>
+      </c>
+      <c r="E35" s="12">
+        <v>0</v>
+      </c>
+      <c r="F35" s="12">
+        <v>1346.65</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G36"/>
+      <c r="A36" s="2">
+        <v>10019034</v>
+      </c>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="2">
-        <v>10031016</v>
-      </c>
-      <c r="B37" s="12">
-        <v>251.75</v>
-      </c>
-      <c r="C37" s="12">
-        <v>16.75</v>
-      </c>
-      <c r="D37" s="12">
-        <v>235</v>
-      </c>
-      <c r="E37" s="12">
-        <v>34.9</v>
-      </c>
-      <c r="F37" s="12">
-        <v>269.89999999999998</v>
-      </c>
-      <c r="G37" s="12" t="s">
-        <v>7</v>
-      </c>
+        <v>10003450</v>
+      </c>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="2">
-        <v>10015790</v>
+        <v>10003450</v>
       </c>
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
@@ -8986,7 +8862,7 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="2">
-        <v>10002298</v>
+        <v>13000295</v>
       </c>
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
@@ -8997,7 +8873,7 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="2">
-        <v>10029636</v>
+        <v>13000295</v>
       </c>
       <c r="B40" s="12"/>
       <c r="C40" s="12"/>
@@ -9008,7 +8884,7 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="2">
-        <v>10001399</v>
+        <v>13000295</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="12"/>
@@ -9019,7 +8895,7 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="2">
-        <v>10001399</v>
+        <v>14000119</v>
       </c>
       <c r="B42" s="12"/>
       <c r="C42" s="12"/>
@@ -9028,38 +8904,38 @@
       <c r="F42" s="12"/>
       <c r="G42" s="12"/>
     </row>
-    <row r="43" spans="1:7" ht="15">
+    <row r="43" spans="1:7">
       <c r="A43" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G43"/>
     </row>
-    <row r="44" spans="1:7" ht="15">
+    <row r="44" spans="1:7">
       <c r="A44" s="2">
         <v>10029636</v>
       </c>
       <c r="B44" s="12">
-        <v>1534</v>
+        <v>549.24</v>
       </c>
       <c r="C44" s="12">
-        <v>16.75</v>
+        <v>36.840000000000003</v>
       </c>
       <c r="D44" s="12">
-        <v>1517.25</v>
+        <v>512.4</v>
       </c>
       <c r="E44" s="12">
         <v>0</v>
       </c>
       <c r="F44" s="12">
-        <v>1517.25</v>
+        <v>512.4</v>
       </c>
       <c r="G44" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" s="2">
-        <v>10015566</v>
+        <v>10033046</v>
       </c>
       <c r="B45" s="12"/>
       <c r="C45" s="12"/>
@@ -9068,9 +8944,9 @@
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
     </row>
-    <row r="46" spans="1:7" ht="14.45" customHeight="1">
+    <row r="46" spans="1:7">
       <c r="A46" s="2">
-        <v>10033046</v>
+        <v>10003450</v>
       </c>
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
@@ -9079,9 +8955,9 @@
       <c r="F46" s="12"/>
       <c r="G46" s="12"/>
     </row>
-    <row r="47" spans="1:7" ht="14.45" customHeight="1">
+    <row r="47" spans="1:7">
       <c r="A47" s="2">
-        <v>10011403</v>
+        <v>13000295</v>
       </c>
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
@@ -9090,31 +8966,38 @@
       <c r="F47" s="12"/>
       <c r="G47" s="12"/>
     </row>
-    <row r="48" spans="1:7" ht="14.45" customHeight="1">
-      <c r="A48" s="2">
-        <v>14000119</v>
-      </c>
-      <c r="B48" s="12"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
-    </row>
-    <row r="49" spans="1:7" ht="14.45" customHeight="1">
+    <row r="48" spans="1:7">
+      <c r="A48" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G48"/>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" s="2">
-        <v>14000119</v>
-      </c>
-      <c r="B49" s="12"/>
-      <c r="C49" s="12"/>
-      <c r="D49" s="12"/>
-      <c r="E49" s="12"/>
-      <c r="F49" s="12"/>
-      <c r="G49" s="12"/>
-    </row>
-    <row r="50" spans="1:7" ht="14.45" customHeight="1">
+        <v>10023698</v>
+      </c>
+      <c r="B49" s="12">
+        <v>331</v>
+      </c>
+      <c r="C49" s="12">
+        <v>31.15</v>
+      </c>
+      <c r="D49" s="12">
+        <v>299.85000000000002</v>
+      </c>
+      <c r="E49" s="12">
+        <v>34.9</v>
+      </c>
+      <c r="F49" s="12">
+        <v>334.75</v>
+      </c>
+      <c r="G49" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" s="2">
-        <v>10011355</v>
+        <v>10003480</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
@@ -9123,9 +9006,9 @@
       <c r="F50" s="12"/>
       <c r="G50" s="12"/>
     </row>
-    <row r="51" spans="1:7" ht="14.45" customHeight="1">
+    <row r="51" spans="1:7">
       <c r="A51" s="2">
-        <v>10003352</v>
+        <v>13000295</v>
       </c>
       <c r="B51" s="12"/>
       <c r="C51" s="12"/>
@@ -9134,45 +9017,673 @@
       <c r="F51" s="12"/>
       <c r="G51" s="12"/>
     </row>
-    <row r="52" spans="1:7" ht="15"/>
+    <row r="52" spans="1:7">
+      <c r="A52" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G52"/>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="2">
+        <v>10001720</v>
+      </c>
+      <c r="B53" s="12">
+        <v>445.99</v>
+      </c>
+      <c r="C53" s="12">
+        <v>36.840000000000003</v>
+      </c>
+      <c r="D53" s="12">
+        <v>409.15</v>
+      </c>
+      <c r="E53" s="12">
+        <v>0</v>
+      </c>
+      <c r="F53" s="12">
+        <v>409.15</v>
+      </c>
+      <c r="G53" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="2">
+        <v>10003450</v>
+      </c>
+      <c r="B54" s="12"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="2">
+        <v>13000295</v>
+      </c>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="2">
+        <v>10005103</v>
+      </c>
+      <c r="B56" s="12"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="12"/>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G57"/>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="2">
+        <v>10011829</v>
+      </c>
+      <c r="B58" s="12">
+        <v>1742.97</v>
+      </c>
+      <c r="C58" s="12">
+        <v>48.22</v>
+      </c>
+      <c r="D58" s="12">
+        <v>1694.75</v>
+      </c>
+      <c r="E58" s="12">
+        <v>0</v>
+      </c>
+      <c r="F58" s="12">
+        <v>1694.75</v>
+      </c>
+      <c r="G58" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" s="2">
+        <v>10008584</v>
+      </c>
+      <c r="B59" s="12"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="12"/>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" s="2">
+        <v>10003450</v>
+      </c>
+      <c r="B60" s="12"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="12"/>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" s="2">
+        <v>10003450</v>
+      </c>
+      <c r="B61" s="12"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="12"/>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="2">
+        <v>10003450</v>
+      </c>
+      <c r="B62" s="12"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="12"/>
+      <c r="F62" s="12"/>
+      <c r="G62" s="12"/>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="2">
+        <v>13000295</v>
+      </c>
+      <c r="B63" s="12"/>
+      <c r="C63" s="12"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="12"/>
+      <c r="F63" s="12"/>
+      <c r="G63" s="12"/>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" s="2">
+        <v>10015188</v>
+      </c>
+      <c r="B64" s="12"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="12"/>
+      <c r="G64" s="12"/>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" s="2">
+        <v>10023115</v>
+      </c>
+      <c r="B65" s="12"/>
+      <c r="C65" s="12"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="12"/>
+      <c r="G65" s="12"/>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G66"/>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" s="2">
+        <v>10019034</v>
+      </c>
+      <c r="B67" s="12">
+        <v>847.98</v>
+      </c>
+      <c r="C67" s="12">
+        <v>73.680000000000007</v>
+      </c>
+      <c r="D67" s="12">
+        <v>774.3</v>
+      </c>
+      <c r="E67" s="12">
+        <v>0</v>
+      </c>
+      <c r="F67" s="12">
+        <v>774.3</v>
+      </c>
+      <c r="G67" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" s="2">
+        <v>10017013</v>
+      </c>
+      <c r="B68" s="12"/>
+      <c r="C68" s="12"/>
+      <c r="D68" s="12"/>
+      <c r="E68" s="12"/>
+      <c r="F68" s="12"/>
+      <c r="G68" s="12"/>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" s="2">
+        <v>10003450</v>
+      </c>
+      <c r="B69" s="12"/>
+      <c r="C69" s="12"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="12"/>
+      <c r="F69" s="12"/>
+      <c r="G69" s="12"/>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" s="2">
+        <v>10003450</v>
+      </c>
+      <c r="B70" s="12"/>
+      <c r="C70" s="12"/>
+      <c r="D70" s="12"/>
+      <c r="E70" s="12"/>
+      <c r="F70" s="12"/>
+      <c r="G70" s="12"/>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" s="2">
+        <v>13000295</v>
+      </c>
+      <c r="B71" s="12"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="12"/>
+      <c r="E71" s="12"/>
+      <c r="F71" s="12"/>
+      <c r="G71" s="12"/>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" s="2">
+        <v>13000295</v>
+      </c>
+      <c r="B72" s="12"/>
+      <c r="C72" s="12"/>
+      <c r="D72" s="12"/>
+      <c r="E72" s="12"/>
+      <c r="F72" s="12"/>
+      <c r="G72" s="12"/>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G73"/>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" s="2">
+        <v>10003450</v>
+      </c>
+      <c r="B74" s="12">
+        <v>1473.96</v>
+      </c>
+      <c r="C74" s="12">
+        <v>147.36000000000001</v>
+      </c>
+      <c r="D74" s="12">
+        <v>1326.6</v>
+      </c>
+      <c r="E74" s="12">
+        <v>0</v>
+      </c>
+      <c r="F74" s="12">
+        <v>1326.6</v>
+      </c>
+      <c r="G74" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" s="2">
+        <v>10003450</v>
+      </c>
+      <c r="B75" s="12"/>
+      <c r="C75" s="12"/>
+      <c r="D75" s="12"/>
+      <c r="E75" s="12"/>
+      <c r="F75" s="12"/>
+      <c r="G75" s="12"/>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76" s="2">
+        <v>10003450</v>
+      </c>
+      <c r="B76" s="12"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="12"/>
+      <c r="G76" s="12"/>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77" s="2">
+        <v>10003450</v>
+      </c>
+      <c r="B77" s="12"/>
+      <c r="C77" s="12"/>
+      <c r="D77" s="12"/>
+      <c r="E77" s="12"/>
+      <c r="F77" s="12"/>
+      <c r="G77" s="12"/>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" s="2">
+        <v>13000295</v>
+      </c>
+      <c r="B78" s="12"/>
+      <c r="C78" s="12"/>
+      <c r="D78" s="12"/>
+      <c r="E78" s="12"/>
+      <c r="F78" s="12"/>
+      <c r="G78" s="12"/>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" s="2">
+        <v>13000295</v>
+      </c>
+      <c r="B79" s="12"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="12"/>
+      <c r="F79" s="12"/>
+      <c r="G79" s="12"/>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" s="2">
+        <v>13000295</v>
+      </c>
+      <c r="B80" s="12"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="12"/>
+      <c r="E80" s="12"/>
+      <c r="F80" s="12"/>
+      <c r="G80" s="12"/>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81" s="2">
+        <v>13000295</v>
+      </c>
+      <c r="B81" s="12"/>
+      <c r="C81" s="12"/>
+      <c r="D81" s="12"/>
+      <c r="E81" s="12"/>
+      <c r="F81" s="12"/>
+      <c r="G81" s="12"/>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82"/>
+      <c r="B82"/>
+      <c r="C82"/>
+      <c r="D82"/>
+      <c r="E82"/>
+      <c r="F82"/>
+      <c r="G82"/>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83"/>
+      <c r="B83"/>
+      <c r="C83"/>
+      <c r="D83"/>
+      <c r="E83"/>
+      <c r="F83"/>
+      <c r="G83"/>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84"/>
+      <c r="B84"/>
+      <c r="C84"/>
+      <c r="D84"/>
+      <c r="E84"/>
+      <c r="F84"/>
+      <c r="G84"/>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85"/>
+      <c r="B85"/>
+      <c r="C85"/>
+      <c r="D85"/>
+      <c r="E85"/>
+      <c r="F85"/>
+      <c r="G85"/>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86"/>
+      <c r="B86"/>
+      <c r="C86"/>
+      <c r="D86"/>
+      <c r="E86"/>
+      <c r="F86"/>
+      <c r="G86"/>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87"/>
+      <c r="B87"/>
+      <c r="C87"/>
+      <c r="D87"/>
+      <c r="E87"/>
+      <c r="F87"/>
+      <c r="G87"/>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88"/>
+      <c r="B88"/>
+      <c r="C88"/>
+      <c r="D88"/>
+      <c r="E88"/>
+      <c r="F88"/>
+      <c r="G88"/>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89"/>
+      <c r="B89"/>
+      <c r="C89"/>
+      <c r="D89"/>
+      <c r="E89"/>
+      <c r="F89"/>
+      <c r="G89"/>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="A90"/>
+      <c r="B90"/>
+      <c r="C90"/>
+      <c r="D90"/>
+      <c r="E90"/>
+      <c r="F90"/>
+      <c r="G90"/>
+    </row>
+    <row r="91" spans="1:7">
+      <c r="A91"/>
+      <c r="B91"/>
+      <c r="C91"/>
+      <c r="D91"/>
+      <c r="E91"/>
+      <c r="F91"/>
+      <c r="G91"/>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="A92"/>
+      <c r="B92"/>
+      <c r="C92"/>
+      <c r="D92"/>
+      <c r="E92"/>
+      <c r="F92"/>
+      <c r="G92"/>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93"/>
+      <c r="B93"/>
+      <c r="C93"/>
+      <c r="D93"/>
+      <c r="E93"/>
+      <c r="F93"/>
+      <c r="G93"/>
+    </row>
+    <row r="94" spans="1:7">
+      <c r="A94"/>
+      <c r="B94"/>
+      <c r="C94"/>
+      <c r="D94"/>
+      <c r="E94"/>
+      <c r="F94"/>
+      <c r="G94"/>
+    </row>
+    <row r="95" spans="1:7">
+      <c r="A95"/>
+      <c r="B95"/>
+      <c r="C95"/>
+      <c r="D95"/>
+      <c r="E95"/>
+      <c r="F95"/>
+      <c r="G95"/>
+    </row>
+    <row r="96" spans="1:7">
+      <c r="A96"/>
+      <c r="B96"/>
+      <c r="C96"/>
+      <c r="D96"/>
+      <c r="E96"/>
+      <c r="F96"/>
+      <c r="G96"/>
+    </row>
+    <row r="97" customFormat="1"/>
+    <row r="98" customFormat="1"/>
+    <row r="99" customFormat="1"/>
+    <row r="100" customFormat="1"/>
+    <row r="101" customFormat="1"/>
+    <row r="102" customFormat="1"/>
+    <row r="103" customFormat="1"/>
+    <row r="104" customFormat="1"/>
+    <row r="105" customFormat="1"/>
+    <row r="106" customFormat="1"/>
+    <row r="107" customFormat="1"/>
+    <row r="108" customFormat="1"/>
+    <row r="109" customFormat="1"/>
+    <row r="110" customFormat="1"/>
+    <row r="111" customFormat="1"/>
+    <row r="112" customFormat="1"/>
+    <row r="113" spans="1:7">
+      <c r="A113"/>
+      <c r="B113"/>
+      <c r="C113"/>
+      <c r="D113"/>
+      <c r="E113"/>
+      <c r="F113"/>
+      <c r="G113"/>
+    </row>
+    <row r="114" spans="1:7">
+      <c r="A114"/>
+      <c r="B114"/>
+      <c r="C114"/>
+      <c r="D114"/>
+      <c r="E114"/>
+      <c r="F114"/>
+      <c r="G114"/>
+    </row>
+    <row r="115" spans="1:7">
+      <c r="A115"/>
+      <c r="B115"/>
+      <c r="C115"/>
+      <c r="D115"/>
+      <c r="E115"/>
+      <c r="F115"/>
+      <c r="G115"/>
+    </row>
+    <row r="116" spans="1:7">
+      <c r="A116"/>
+      <c r="B116"/>
+      <c r="C116"/>
+      <c r="D116"/>
+      <c r="E116"/>
+      <c r="F116"/>
+      <c r="G116"/>
+    </row>
+    <row r="117" spans="1:7">
+      <c r="A117"/>
+      <c r="B117"/>
+      <c r="C117"/>
+      <c r="D117"/>
+      <c r="E117"/>
+      <c r="F117"/>
+      <c r="G117"/>
+    </row>
+    <row r="118" spans="1:7">
+      <c r="A118"/>
+      <c r="B118"/>
+      <c r="C118"/>
+      <c r="D118"/>
+      <c r="E118"/>
+      <c r="F118"/>
+      <c r="G118"/>
+    </row>
+    <row r="119" spans="1:7">
+      <c r="A119"/>
+      <c r="B119"/>
+      <c r="C119"/>
+      <c r="D119"/>
+      <c r="E119"/>
+      <c r="F119"/>
+      <c r="G119"/>
+    </row>
+    <row r="120" spans="1:7">
+      <c r="A120"/>
+      <c r="B120"/>
+      <c r="C120"/>
+      <c r="D120"/>
+      <c r="E120"/>
+      <c r="F120"/>
+      <c r="G120"/>
+    </row>
+    <row r="121" spans="1:7">
+      <c r="G121"/>
+    </row>
+    <row r="122" spans="1:7">
+      <c r="G122"/>
+    </row>
+    <row r="123" spans="1:7">
+      <c r="G123"/>
+    </row>
+    <row r="124" spans="1:7">
+      <c r="G124"/>
+    </row>
   </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="B2:B9"/>
-    <mergeCell ref="C2:C9"/>
-    <mergeCell ref="D2:D9"/>
-    <mergeCell ref="E2:E9"/>
-    <mergeCell ref="F2:F9"/>
-    <mergeCell ref="B20:B27"/>
-    <mergeCell ref="C20:C27"/>
-    <mergeCell ref="D20:D27"/>
-    <mergeCell ref="E20:E27"/>
-    <mergeCell ref="F20:F27"/>
-    <mergeCell ref="B11:B18"/>
-    <mergeCell ref="C11:C18"/>
-    <mergeCell ref="D11:D18"/>
-    <mergeCell ref="E11:E18"/>
-    <mergeCell ref="F11:F18"/>
-    <mergeCell ref="B29:B35"/>
-    <mergeCell ref="C29:C35"/>
-    <mergeCell ref="D29:D35"/>
-    <mergeCell ref="E29:E35"/>
-    <mergeCell ref="F29:F35"/>
-    <mergeCell ref="B37:B42"/>
-    <mergeCell ref="C37:C42"/>
-    <mergeCell ref="D37:D42"/>
-    <mergeCell ref="E37:E42"/>
-    <mergeCell ref="F37:F42"/>
-    <mergeCell ref="G29:G35"/>
-    <mergeCell ref="G37:G42"/>
-    <mergeCell ref="G2:G9"/>
-    <mergeCell ref="G11:G18"/>
-    <mergeCell ref="G20:G27"/>
-    <mergeCell ref="G44:G51"/>
-    <mergeCell ref="B44:B51"/>
-    <mergeCell ref="C44:C51"/>
-    <mergeCell ref="D44:D51"/>
-    <mergeCell ref="E44:E51"/>
-    <mergeCell ref="F44:F51"/>
+  <mergeCells count="72">
+    <mergeCell ref="G2:G6"/>
+    <mergeCell ref="G74:G81"/>
+    <mergeCell ref="G67:G72"/>
+    <mergeCell ref="G58:G65"/>
+    <mergeCell ref="G53:G56"/>
+    <mergeCell ref="G49:G51"/>
+    <mergeCell ref="G44:G47"/>
+    <mergeCell ref="G35:G42"/>
+    <mergeCell ref="G26:G33"/>
+    <mergeCell ref="G17:G24"/>
+    <mergeCell ref="G12:G15"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="F53:F56"/>
+    <mergeCell ref="E53:E56"/>
+    <mergeCell ref="D53:D56"/>
+    <mergeCell ref="C53:C56"/>
+    <mergeCell ref="B53:B56"/>
+    <mergeCell ref="B67:B72"/>
+    <mergeCell ref="C67:C72"/>
+    <mergeCell ref="D67:D72"/>
+    <mergeCell ref="E67:E72"/>
+    <mergeCell ref="F67:F72"/>
+    <mergeCell ref="B74:B81"/>
+    <mergeCell ref="C74:C81"/>
+    <mergeCell ref="D74:D81"/>
+    <mergeCell ref="E74:E81"/>
+    <mergeCell ref="F74:F81"/>
+    <mergeCell ref="B58:B65"/>
+    <mergeCell ref="C58:C65"/>
+    <mergeCell ref="D58:D65"/>
+    <mergeCell ref="E58:E65"/>
+    <mergeCell ref="F58:F65"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="C44:C47"/>
+    <mergeCell ref="D44:D47"/>
+    <mergeCell ref="E44:E47"/>
+    <mergeCell ref="F44:F47"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="D49:D51"/>
+    <mergeCell ref="E49:E51"/>
+    <mergeCell ref="F49:F51"/>
+    <mergeCell ref="B26:B33"/>
+    <mergeCell ref="C26:C33"/>
+    <mergeCell ref="D26:D33"/>
+    <mergeCell ref="E26:E33"/>
+    <mergeCell ref="F26:F33"/>
+    <mergeCell ref="B35:B42"/>
+    <mergeCell ref="C35:C42"/>
+    <mergeCell ref="D35:D42"/>
+    <mergeCell ref="E35:E42"/>
+    <mergeCell ref="F35:F42"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="F12:F15"/>
+    <mergeCell ref="B17:B24"/>
+    <mergeCell ref="C17:C24"/>
+    <mergeCell ref="D17:D24"/>
+    <mergeCell ref="E17:E24"/>
+    <mergeCell ref="F17:F24"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="E2:E6"/>
+    <mergeCell ref="F2:F6"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="F8:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>